<commit_message>
comparison S toc analysis (preliminary)
</commit_message>
<xml_diff>
--- a/data/raw_lab_data/Fuhrberg CHNS.xlsx
+++ b/data/raw_lab_data/Fuhrberg CHNS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FFA_colexperiment/data/raw_lab_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B415DCD6-A61D-4B49-86A6-12F7BD43076A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4B69E2-B4BD-E047-A6F8-40ABAA0D74C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="740" windowWidth="28260" windowHeight="16680" xr2:uid="{D8F29EDB-924B-AB45-BE47-83C51CA64082}"/>
   </bookViews>
@@ -990,7 +990,7 @@
   <dimension ref="B1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>